<commit_message>
updates for final thesis
</commit_message>
<xml_diff>
--- a/WGCNA/Module_GO_Overview.xlsx
+++ b/WGCNA/Module_GO_Overview.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Melissa/Desktop/GitHub/RNAseq_allsites_Barshisreference/WGCNA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC758B54-D833-CF4B-B860-FFDE3C4EC5BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB38D12-CEBB-6B47-8F26-7EC595AEC69B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9520" yWindow="460" windowWidth="20460" windowHeight="16540" xr2:uid="{E1D4700D-1A04-844D-9E39-5AFFC62DDCE4}"/>
+    <workbookView xWindow="360" yWindow="460" windowWidth="24720" windowHeight="16540" activeTab="2" xr2:uid="{E1D4700D-1A04-844D-9E39-5AFFC62DDCE4}"/>
   </bookViews>
   <sheets>
     <sheet name="simplified GO terms" sheetId="3" r:id="rId1"/>
-    <sheet name="all info" sheetId="1" r:id="rId2"/>
-    <sheet name="info" sheetId="2" r:id="rId3"/>
+    <sheet name="all info- p.adj then by p value" sheetId="4" r:id="rId2"/>
+    <sheet name="all info" sheetId="1" r:id="rId3"/>
+    <sheet name="info" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="118">
   <si>
     <t>Analysis</t>
   </si>
@@ -227,39 +228,21 @@
     <t>from MWU_BP/MF_signiffile with lowest p value only if adj p &lt; 0.05</t>
   </si>
   <si>
-    <t>Metabolic process</t>
-  </si>
-  <si>
-    <t>Response to stress</t>
-  </si>
-  <si>
-    <t>Cellular component organization</t>
+    <t>RNA processing</t>
   </si>
   <si>
     <t>Translation</t>
   </si>
   <si>
-    <t>Downregulation of multi-organism process</t>
-  </si>
-  <si>
-    <t>Ion transport</t>
-  </si>
-  <si>
     <t>Downregulation of catabolic process</t>
   </si>
   <si>
     <t>Proteasome binding</t>
   </si>
   <si>
-    <t>Oxidoreductase activity</t>
-  </si>
-  <si>
     <t>Transferase activity</t>
   </si>
   <si>
-    <t>Glucosidase activity</t>
-  </si>
-  <si>
     <t>Hydrolase activity</t>
   </si>
   <si>
@@ -267,13 +250,154 @@
   </si>
   <si>
     <t xml:space="preserve">from MWU_BP/MF_signiffile with lowest p value only if adj p &lt; 0.05. sort by p value and choose lowest </t>
+  </si>
+  <si>
+    <t>calcium ion transport</t>
+  </si>
+  <si>
+    <t>receptor signaling complex scaffold activity</t>
+  </si>
+  <si>
+    <t>membrane docking</t>
+  </si>
+  <si>
+    <t>activation of MAPKK activity</t>
+  </si>
+  <si>
+    <t>gene silencing by RNA</t>
+  </si>
+  <si>
+    <t>positive regulation of developmental process</t>
+  </si>
+  <si>
+    <t>vesicle-mediated transport</t>
+  </si>
+  <si>
+    <t>spliceosomal complex assembly</t>
+  </si>
+  <si>
+    <t>sodium channel activity</t>
+  </si>
+  <si>
+    <t>MAP kinase kinase kinase activity</t>
+  </si>
+  <si>
+    <t>protein kinase C binding</t>
+  </si>
+  <si>
+    <t>phospholipase binding</t>
+  </si>
+  <si>
+    <t>sequence-specific DNA binding</t>
+  </si>
+  <si>
+    <t>immune response</t>
+  </si>
+  <si>
+    <t>NA redo this and BP?</t>
+  </si>
+  <si>
+    <t>small molecule metabolic process</t>
+  </si>
+  <si>
+    <t>intracellular signal transduction</t>
+  </si>
+  <si>
+    <t>Immune response</t>
+  </si>
+  <si>
+    <t>Signaling adaptor activity</t>
+  </si>
+  <si>
+    <t>Developmental processes</t>
+  </si>
+  <si>
+    <t>DNA binding</t>
+  </si>
+  <si>
+    <t>Kinase binding</t>
+  </si>
+  <si>
+    <t>Enzyme binding</t>
+  </si>
+  <si>
+    <t>RNA splicing</t>
+  </si>
+  <si>
+    <t>Membrane docking</t>
+  </si>
+  <si>
+    <t>Ion channel activity</t>
+  </si>
+  <si>
+    <t>Transport</t>
+  </si>
+  <si>
+    <t>Signaling</t>
+  </si>
+  <si>
+    <t>superoxide anion generation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reactive oxygen species </t>
+  </si>
+  <si>
+    <t>DNA biosynthetic process</t>
+  </si>
+  <si>
+    <t>DNA metabolic process</t>
+  </si>
+  <si>
+    <t>Small molecule metabolic process</t>
+  </si>
+  <si>
+    <t>External encapsulating structure organization</t>
+  </si>
+  <si>
+    <t>one-carbon metabolic process</t>
+  </si>
+  <si>
+    <t>negative regulation of cytokine production</t>
+  </si>
+  <si>
+    <t>Cellular metabolic process</t>
+  </si>
+  <si>
+    <t>Downregulation of cytokine production</t>
+  </si>
+  <si>
+    <t>MAPK Activity</t>
+  </si>
+  <si>
+    <t>Gene silencing by RNA</t>
+  </si>
+  <si>
+    <t>Activation of MAPKK activity</t>
+  </si>
+  <si>
+    <t>Calcium ion transport</t>
+  </si>
+  <si>
+    <t>Inorganic cation transport</t>
+  </si>
+  <si>
+    <t>amino acid activation</t>
+  </si>
+  <si>
+    <t>Amino acid activation</t>
+  </si>
+  <si>
+    <t>DNA integration</t>
+  </si>
+  <si>
+    <t>NA redo this ?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -289,13 +413,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -319,7 +456,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -334,12 +471,22 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF57BF"/>
+      <color rgb="FFFF3DAE"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -650,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A50BA4FA-CDDD-E546-A1ED-CD65C16297F1}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -662,8 +809,8 @@
     <col min="4" max="4" width="25.5" style="3" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="3"/>
     <col min="6" max="6" width="16.83203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="36.6640625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="23.5" style="3" customWidth="1"/>
+    <col min="7" max="7" width="40.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
@@ -727,13 +874,13 @@
         <v>9</v>
       </c>
       <c r="E3" s="3">
-        <v>0.97</v>
+        <v>-0.97</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>63</v>
+      <c r="G3" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -755,6 +902,9 @@
       <c r="F4" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="G4" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
@@ -775,6 +925,9 @@
       <c r="F5" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="G5" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
@@ -795,6 +948,9 @@
       <c r="F6" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="G6" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
@@ -815,8 +971,8 @@
       <c r="F7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="5" t="s">
-        <v>64</v>
+      <c r="G7" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -858,6 +1014,9 @@
       <c r="F9" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="G9" s="3" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
@@ -898,6 +1057,9 @@
       <c r="F11" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="G11" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
@@ -918,6 +1080,9 @@
       <c r="F12" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="G12" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
@@ -938,7 +1103,9 @@
       <c r="F13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H13" s="5"/>
+      <c r="G13" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
@@ -959,11 +1126,11 @@
       <c r="F14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G14" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>74</v>
+      <c r="G14" t="s">
+        <v>104</v>
+      </c>
+      <c r="H14" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -985,11 +1152,11 @@
       <c r="F15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>74</v>
+      <c r="G15" t="s">
+        <v>104</v>
+      </c>
+      <c r="H15" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -1011,11 +1178,11 @@
       <c r="F16" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G16" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>73</v>
+      <c r="G16" t="s">
+        <v>64</v>
+      </c>
+      <c r="H16" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -1037,11 +1204,11 @@
       <c r="F17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="G17" t="s">
+        <v>88</v>
+      </c>
+      <c r="H17" t="s">
         <v>67</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -1063,11 +1230,8 @@
       <c r="F18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G18" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>72</v>
+      <c r="H18" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -1089,11 +1253,8 @@
       <c r="F19" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G19" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>49</v>
+      <c r="H19" s="6" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -1115,11 +1276,8 @@
       <c r="F20" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G20" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>71</v>
+      <c r="G20" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -1141,11 +1299,11 @@
       <c r="F21" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G21" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>70</v>
+      <c r="G21" t="s">
+        <v>65</v>
+      </c>
+      <c r="H21" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -1167,6 +1325,12 @@
       <c r="F22" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="G22" t="s">
+        <v>112</v>
+      </c>
+      <c r="H22" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
@@ -1187,6 +1351,12 @@
       <c r="F23" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="G23" t="s">
+        <v>90</v>
+      </c>
+      <c r="H23" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
@@ -1207,6 +1377,12 @@
       <c r="F24" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="G24" t="s">
+        <v>110</v>
+      </c>
+      <c r="H24" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
@@ -1227,6 +1403,12 @@
       <c r="F25" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="G25" t="s">
+        <v>63</v>
+      </c>
+      <c r="H25" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
@@ -1247,6 +1429,12 @@
       <c r="F26" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="G26" t="s">
+        <v>110</v>
+      </c>
+      <c r="H26" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
@@ -1267,6 +1455,12 @@
       <c r="F27" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="G27" t="s">
+        <v>63</v>
+      </c>
+      <c r="H27" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
@@ -1288,7 +1482,7 @@
         <v>23</v>
       </c>
       <c r="G28" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -1310,6 +1504,12 @@
       <c r="F29" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="G29" t="s">
+        <v>95</v>
+      </c>
+      <c r="H29" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
@@ -1330,6 +1530,9 @@
       <c r="F30" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="G30" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
@@ -1349,6 +1552,12 @@
       </c>
       <c r="F31" s="3" t="s">
         <v>23</v>
+      </c>
+      <c r="G31" t="s">
+        <v>111</v>
+      </c>
+      <c r="H31" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1357,11 +1566,809 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3A6AFE7-A255-0E47-ACA1-0E6A54FF8193}">
+  <dimension ref="A1:H31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H27" sqref="H27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="26" style="3" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="3"/>
+    <col min="6" max="6" width="7.83203125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="39.33203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="52" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="4">
+        <v>117</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="4">
+        <v>-0.32</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3">
+        <v>6036</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.97</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="3">
+        <v>125</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.36</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3">
+        <v>172</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="3">
+        <v>391</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.42</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="3">
+        <v>3969</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="3">
+        <v>291</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.54</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="3">
+        <v>112</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.33</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="3">
+        <v>691</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.64</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="3">
+        <v>150</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.44</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="3">
+        <v>267</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="3">
+        <v>174</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.43</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="3">
+        <v>190</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="3">
+        <v>-0.46</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" t="s">
+        <v>60</v>
+      </c>
+      <c r="H14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="3">
+        <v>190</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.72</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" t="s">
+        <v>60</v>
+      </c>
+      <c r="H15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="3">
+        <v>495</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" t="s">
+        <v>50</v>
+      </c>
+      <c r="H16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="3">
+        <v>117</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0.63</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" t="s">
+        <v>84</v>
+      </c>
+      <c r="H17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="3">
+        <v>267</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="3">
+        <v>406</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="3">
+        <v>69</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" t="s">
+        <v>54</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="3">
+        <v>280</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" t="s">
+        <v>56</v>
+      </c>
+      <c r="H21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="3">
+        <v>412</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" s="3">
+        <v>-0.51</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" t="s">
+        <v>71</v>
+      </c>
+      <c r="H22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="3">
+        <v>762</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="3">
+        <v>-0.55000000000000004</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23" t="s">
+        <v>76</v>
+      </c>
+      <c r="H23" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="3">
+        <v>256</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" s="3">
+        <v>-0.45</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" t="s">
+        <v>75</v>
+      </c>
+      <c r="H24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="3">
+        <v>600</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25" s="3">
+        <v>-0.45</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G25" t="s">
+        <v>63</v>
+      </c>
+      <c r="H25" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="3">
+        <v>256</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" s="3">
+        <v>0.86</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26" t="s">
+        <v>75</v>
+      </c>
+      <c r="H26" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="3">
+        <v>600</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" s="3">
+        <v>0.66</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G27" t="s">
+        <v>63</v>
+      </c>
+      <c r="H27" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="3">
+        <v>627</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" s="3">
+        <v>0.62</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G28" t="s">
+        <v>78</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" s="3">
+        <v>472</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E29" s="3">
+        <v>0.54</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G29" t="s">
+        <v>73</v>
+      </c>
+      <c r="H29" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="3">
+        <v>143</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" s="3">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G30" t="s">
+        <v>77</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="3">
+        <v>210</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E31" s="3">
+        <v>0.52</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G31" t="s">
+        <v>74</v>
+      </c>
+      <c r="H31" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FE604BB-6F21-2C4E-8CC1-750CA0D003A7}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1889,6 +2896,12 @@
       <c r="F22" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="G22" t="s">
+        <v>71</v>
+      </c>
+      <c r="H22" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
@@ -1929,6 +2942,9 @@
       <c r="F24" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="G24" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
@@ -1949,6 +2965,9 @@
       <c r="F25" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="G25" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
@@ -1989,6 +3008,9 @@
       <c r="F27" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="G27" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
@@ -2009,6 +3031,12 @@
       <c r="F28" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="G28" t="s">
+        <v>69</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
@@ -2029,6 +3057,9 @@
       <c r="F29" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="G29" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
@@ -2068,6 +3099,9 @@
       </c>
       <c r="F31" s="3" t="s">
         <v>23</v>
+      </c>
+      <c r="G31" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -2075,18 +3109,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB3E6566-9AD6-184D-90FB-6F2749976665}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="51.5" customWidth="1"/>
-    <col min="2" max="2" width="83" customWidth="1"/>
+    <col min="2" max="2" width="88.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="76.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2106,7 +3140,7 @@
         <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
         <v>62</v>

</xml_diff>